<commit_message>
[UPD] Add automatic generation of significant ROI SDI tables in 02_SDI_consensus and 06_Reproducibility
</commit_message>
<xml_diff>
--- a/SDI_comparison_table_EPvsCTRL.xlsx
+++ b/SDI_comparison_table_EPvsCTRL.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,14 +504,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>lateralorbitofrontal_2</t>
+          <t>rostralanteriorcingulate_1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>-0.61</v>
+      </c>
       <c r="F4" t="n">
-        <v>-1.14</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="5">
@@ -520,13 +522,13 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>rostralanteriorcingulate_1</t>
+          <t>parahippocampal_1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>-0.61</v>
+        <v>-0.91</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
@@ -536,15 +538,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>caudalanteriorcingulate_1</t>
+          <t>insula_1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>-0.71</v>
-      </c>
+      <c r="E6" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -552,16 +554,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>parahippocampal_1</t>
+          <t>Right-Amygdala</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>-0.91</v>
+        <v>-2.34</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.79</v>
+        <v>-2.25</v>
       </c>
     </row>
     <row r="8">
@@ -570,15 +572,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>insula_1</t>
+          <t>Right-Hippocampus</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+        <v>-0.93</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.66</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -586,17 +590,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Right-Amygdala</t>
+          <t>lateralorbitofrontal_1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>-2.34</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-2.28</v>
-      </c>
+        <v>-0.64</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -604,17 +606,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Right-Hippocampus</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>-0.93</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-0.68</v>
-      </c>
+          <t>parstriangularis_1</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.12</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-2.36</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -622,14 +624,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>lateralorbitofrontal_1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>parsopercularis_1</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-1.28</v>
+      </c>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>-0.64</v>
-      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -638,17 +640,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>parstriangularis_1</t>
+          <t>parahippocampal_1</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-2.12</v>
+        <v>-1.59</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.36</v>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+        <v>-1.91</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.88</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-0.91</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -656,13 +662,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>parsopercularis_1</t>
+          <t>Left-Amygdala</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-1.28</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
+        <v>-2.11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-2.15</v>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -672,56 +680,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>parahippocampal_1</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>-1.59</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-1.91</v>
-      </c>
+          <t>Left-Hippocampus</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>-0.88</v>
+        <v>-0.2</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.89</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Left-Amygdala</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>-2.11</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-2.15</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Left-Hippocampus</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-0.12</v>
+        <v>-0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>